<commit_message>
v5 Updated list checkboxes
</commit_message>
<xml_diff>
--- a/app/assets/img/Spotlight - Combined checks.xlsx
+++ b/app/assets/img/Spotlight - Combined checks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\black\Documents\prototypes\confi-prototypes\app\assets\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD5B984-E963-42D5-B24D-057C31E4A63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256CE4CA-A874-4ED3-BB3D-4F059C2C561A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="372" windowWidth="38208" windowHeight="16500" tabRatio="810" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="372" windowWidth="38208" windowHeight="16500" tabRatio="810" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="14" r:id="rId1"/>
@@ -26,12 +26,25 @@
     <sheet name="5.1 Individual adverse media" sheetId="12" r:id="rId11"/>
     <sheet name="5.2 Individual PEPs" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23361" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23363" uniqueCount="531">
   <si>
     <r>
       <rPr>
@@ -1355,12 +1368,6 @@
     <t>Number of applications submitted</t>
   </si>
   <si>
-    <t>Sole directors may indicate high levels of control, lack of segregation of duties and too much autonomy on spend.
-Where a company has fewer than 2 directors display: RED
-Where a company has 2 directors display: AMBER
-Where a company has 3 directors display: GREEN</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1369,12 +1376,6 @@
       </rPr>
       <t>Number of current directors</t>
     </r>
-  </si>
-  <si>
-    <t>Organisations may have been set up for the sole purpose of receiving a grant. Newly-formed charities will be inexperienced stewards of grant funding.
-Where an organisation age is less than 1 year display: RED
-Where an organisation age is between 1 year and 2 years display: AMBER
-Where an organisation age is 2 years and above display: GREEN</t>
   </si>
   <si>
     <r>
@@ -1444,11 +1445,6 @@
     </r>
   </si>
   <si>
-    <t>Operational Status: This shows the activity status of the applicant organisation. You should consider whether to fund an organisation that is not active.
-RED: Where an organisation has any status other than "Active"
-GREEN: Where an organisation is "Active"</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1457,12 +1453,6 @@
       </rPr>
       <t>Operational Status</t>
     </r>
-  </si>
-  <si>
-    <t>Applicants may be over-reliant on grant funding. This indicator compares the value of the grant applied for to the company’s latest declared turnover.
-Where ratio of grant funding to turnover is over 50% display: RED
-Where ratio of grant funding to turnover is between 25% and 50% display: AMBER 
-Where ratio of grant funding to turnover is less that 25% display: GREEN</t>
   </si>
   <si>
     <r>
@@ -1475,12 +1465,6 @@
     </r>
   </si>
   <si>
-    <t>Applicants may be over-reliant on grant funding. This indicator compares the value of the grant applied for to the company's latest declared net worth.
-Where ratio of grant funding to net worth is over 75% or is negative, display: RED
-Where ratio of grant funding to net worth is between 50% and 75%, display: AMBER
-Where ratio of grant funding to net worth is less than 50%, display: GREEN</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1489,12 +1473,6 @@
       </rPr>
       <t>Net worth vs grant amount</t>
     </r>
-  </si>
-  <si>
-    <t>Applicants may be over-reliant on grant funding. This indicator compares the value of the grant applied for to the company’s most recent credit limit.
-Where ratio of grant to credit limit is over 50% display: RED
-Where ratio of grant to credit limit is between 25% and 50% display: AMBER
-Where ratio of grant to credit limit is less than 25% display: GREEN</t>
   </si>
   <si>
     <r>
@@ -1540,11 +1518,6 @@
     </r>
   </si>
   <si>
-    <t>One or more directors with an overseas address may mean that the organisation/entity applying for the grant may not have a principal core business in the UK. 
-Where more than 25% of directors have overseas addresses display: RED 
-Where less than 25% of directors have overseas addresses display: GREEN</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1553,16 +1526,6 @@
       </rPr>
       <t>Percentage of directors registered as overseas residents</t>
     </r>
-  </si>
-  <si>
-    <t>Risk: The Risk rating provides information on the potential risk of poor financial stewardship. This indicator includes information on: 
-• Minimum data 
-• High risk parents 
-• Detrimental legal events 
-• Possible fraudulent activity
-Where the commercial Delphi band is "Higher than average risk" or "High risk" display: RED 
-Where the commercial Delphi band is "Lower than average risk" display: AMBER 
-Where the commercial Delphi band is "Minimum risk" display: GREEN</t>
   </si>
   <si>
     <r>
@@ -1596,11 +1559,6 @@
     </r>
   </si>
   <si>
-    <t>Accounts are deemed qualified by an auditor when there are certain doubts or disagreements with the audited firm’s management about certain items. These disagreements are an indicator of financial irregularity within the entity. 
-Where audit qualification is "Major qualification (Risk index suppressed)" or "Major qualification (Risk index not suppressed)" display: RED 
-Where audit qualification is "No qualification" display: GREEN</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1609,18 +1567,6 @@
       </rPr>
       <t>Are accounts qualified?</t>
     </r>
-  </si>
-  <si>
-    <t>Risk: The Failure score is an analytical tool designed to highlight the strength, performance and creditworthiness of a entity in a single score. The score ranges from 0 to 100 with the lowest scoring companies carrying the highest risk. 
-Some data elements used to calculate the score include:  
-• Company type 
-• Age of business 
-• Lawsuits, liens, judgments 
-• Net worth 
-• Trade data 
-Where a company has a credit score below 25, display: RED 
-Where a company has a credit score between 25 and 50, display: AMBER 
-Where a company has a credit score over 50, display: GREEN</t>
   </si>
   <si>
     <r>
@@ -1633,12 +1579,6 @@
     </r>
   </si>
   <si>
-    <t>A high number of resignations in the last 12 months, especially relative to the number of current directors, may be indicative of poor company performance.
-Where the number of resignations in the past 12 months in a company is more than 75% of the total number of directors, display: RED 
-Where the number of resignations in the past 12 months in a company is between 25 and 75% of the total number of directors, display: AMBER
-Where the number of resignations in the past 12 months in a company is less than 25% of the total number of directors, display: GREEN</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1649,12 +1589,6 @@
     </r>
   </si>
   <si>
-    <t>A high number of appointments in the last 12 months, especially relative to the number of current directors, may be indicative of poor company performance. 
-Where the number of appointments in the past 12 months in a company is more than 75% of the total number of directors, display: RED 
-Where the number of appointments in the past 12 months in a company is between 25 and 75% of the total number of directors, display: AMBER 
-Where the number of appointments in the past 12 months in a company is less than 25% of the total number of directors, display: GREEN</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1662,16 +1596,6 @@
         <rFont val="Calibri"/>
       </rPr>
       <t>Number of directors appointed in the past 12 months vs number of current directors</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Description &amp; Risk</t>
     </r>
   </si>
   <si>
@@ -2185,6 +2109,91 @@
   <si>
     <t xml:space="preserve">             &lt;-- SAME AS 1.2                                                            </t>
   </si>
+  <si>
+    <t>RAG name</t>
+  </si>
+  <si>
+    <t>Description &amp; Risk</t>
+  </si>
+  <si>
+    <t>A high number of appointments in the last 12 months, especially relative to the number of current directors, may be indicative of poor company performance. 
+- Where the number of appointments in the past 12 months in a company is more than 75% of the total number of directors, display: RED 
+- Where the number of appointments in the past 12 months in a company is between 25 and 75% of the total number of directors, display: AMBER 
+- Where the number of appointments in the past 12 months in a company is less than 25% of the total number of directors, display: GREEN</t>
+  </si>
+  <si>
+    <t>A high number of resignations in the last 12 months, especially relative to the number of current directors, may be indicative of poor company performance.
+- Where the number of resignations in the past 12 months in a company is more than 75% of the total number of directors, display: RED 
+- Where the number of resignations in the past 12 months in a company is between 25 and 75% of the total number of directors, display: AMBER
+- Where the number of resignations in the past 12 months in a company is less than 25% of the total number of directors, display: GREEN</t>
+  </si>
+  <si>
+    <t>Risk: The Failure score is an analytical tool designed to highlight the strength, performance and creditworthiness of a entity in a single score. The score ranges from 0 to 100 with the lowest scoring companies carrying the highest risk. 
+Some data elements used to calculate the score include:  
+• Company type 
+• Age of business 
+• Lawsuits, liens, judgments 
+• Net worth 
+• Trade data 
+- Where a company has a credit score below 25, display: RED 
+- Where a company has a credit score between 25 and 50, display: AMBER 
+- Where a company has a credit score over 50, display: GREEN</t>
+  </si>
+  <si>
+    <t>Accounts are deemed qualified by an auditor when there are certain doubts or disagreements with the audited firm’s management about certain items. These disagreements are an indicator of financial irregularity within the entity. 
+- Where audit qualification is "Major qualification (Risk index suppressed)" or "Major qualification (Risk index not suppressed)" display: RED 
+- Where audit qualification is "No qualification" display: GREEN</t>
+  </si>
+  <si>
+    <t>Risk: The Risk rating provides information on the potential risk of poor financial stewardship. This indicator includes information on: 
+• Minimum data 
+• High risk parents 
+• Detrimental legal events 
+• Possible fraudulent activity
+- Where the commercial Delphi band is "Higher than average risk" or "High risk" display: RED 
+- Where the commercial Delphi band is "Lower than average risk" display: AMBER 
+- Where the commercial Delphi band is "Minimum risk" display: GREEN</t>
+  </si>
+  <si>
+    <t>One or more directors with an overseas address may mean that the organisation/entity applying for the grant may not have a principal core business in the UK. 
+- Where more than 25% of directors have overseas addresses display: RED 
+- Where less than 25% of directors have overseas addresses display: GREEN</t>
+  </si>
+  <si>
+    <t>Applicants may be over-reliant on grant funding. This indicator compares the value of the grant applied for to the company’s most recent credit limit.
+- Where ratio of grant to credit limit is over 50% display: RED
+- Where ratio of grant to credit limit is between 25% and 50% display: AMBER
+- Where ratio of grant to credit limit is less than 25% display: GREEN</t>
+  </si>
+  <si>
+    <t>Applicants may be over-reliant on grant funding. This indicator compares the value of the grant applied for to the company's latest declared net worth.
+- Where ratio of grant funding to net worth is over 75% or is negative, display: RED
+- Where ratio of grant funding to net worth is between 50% and 75%, display: AMBER
+- Where ratio of grant funding to net worth is less than 50%, display: GREEN</t>
+  </si>
+  <si>
+    <t>Applicants may be over-reliant on grant funding. This indicator compares the value of the grant applied for to the company’s latest declared turnover.
+- Where ratio of grant funding to turnover is over 50% display: RED
+- Where ratio of grant funding to turnover is between 25% and 50% display: AMBER 
+- Where ratio of grant funding to turnover is less that 25% display: GREEN</t>
+  </si>
+  <si>
+    <t>Operational Status: This shows the activity status of the applicant organisation. You should consider whether to fund an organisation that is not active.
+- RED: Where an organisation has any status other than "Active"
+- GREEN: Where an organisation is "Active"</t>
+  </si>
+  <si>
+    <t>Organisations may have been set up for the sole purpose of receiving a grant. Newly-formed charities will be inexperienced stewards of grant funding.
+- Where an organisation age is less than 1 year display: RED
+- Where an organisation age is between 1 year and 2 years display: AMBER
+- Where an organisation age is 2 years and above display: GREEN</t>
+  </si>
+  <si>
+    <t>Sole directors may indicate high levels of control, lack of segregation of duties and too much autonomy on spend.
+- Where a company has fewer than 2 directors display: RED
+- Where a company has 2 directors display: AMBER
+- Where a company has 3 directors display: GREEN</t>
+  </si>
 </sst>
 </file>
 
@@ -2193,7 +2202,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2255,8 +2264,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2311,8 +2328,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -2320,11 +2343,114 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2351,8 +2477,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3504,87 +3650,87 @@
   <sheetData>
     <row r="2" spans="2:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="16" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="21" x14ac:dyDescent="0.4">
       <c r="B4" s="15" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="21" x14ac:dyDescent="0.4">
       <c r="B9" s="15" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="21" x14ac:dyDescent="0.4">
       <c r="B13" s="15" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="21" x14ac:dyDescent="0.4">
       <c r="B18" s="15" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="21" x14ac:dyDescent="0.4">
       <c r="B21" s="15" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -3654,7 +3800,7 @@
         <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>492</v>
+        <v>479</v>
       </c>
       <c r="C2" t="s">
         <v>77</v>
@@ -3698,7 +3844,7 @@
         <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="C3" t="s">
         <v>77</v>
@@ -3954,7 +4100,7 @@
         <v>77</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -3971,16 +4117,16 @@
         <v>98</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>102</v>
@@ -3995,54 +4141,54 @@
         <v>105</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="B10" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="C10" s="14">
         <v>45593.50949074074</v>
       </c>
       <c r="D10" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
       <c r="E10" t="s">
         <v>190</v>
       </c>
       <c r="F10" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="G10" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="H10">
         <v>1000</v>
       </c>
       <c r="I10" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
       <c r="J10" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="K10" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="L10" t="s">
         <v>223</v>
       </c>
       <c r="M10" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -4116,7 +4262,7 @@
         <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
       <c r="C2" t="s">
         <v>77</v>
@@ -4160,7 +4306,7 @@
         <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="C3" t="s">
         <v>77</v>
@@ -4416,7 +4562,7 @@
         <v>77</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -4430,19 +4576,19 @@
         <v>96</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>102</v>
@@ -4457,10 +4603,10 @@
         <v>105</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -4468,22 +4614,22 @@
         <v>162</v>
       </c>
       <c r="B10" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="C10" s="14">
         <v>45582.54724537037</v>
       </c>
       <c r="D10" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
       <c r="E10" t="s">
         <v>190</v>
       </c>
       <c r="F10" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="G10" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -4498,13 +4644,13 @@
         <v>223</v>
       </c>
       <c r="L10" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="M10" t="s">
         <v>223</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -4512,22 +4658,22 @@
         <v>162</v>
       </c>
       <c r="B11" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="C11" s="14">
         <v>45582.54724537037</v>
       </c>
       <c r="D11" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="E11" t="s">
         <v>190</v>
       </c>
       <c r="F11" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="G11" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -4542,13 +4688,13 @@
         <v>223</v>
       </c>
       <c r="L11" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="M11" t="s">
         <v>223</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -4556,22 +4702,22 @@
         <v>162</v>
       </c>
       <c r="B12" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="C12" s="14">
         <v>45582.54724537037</v>
       </c>
       <c r="D12" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
       <c r="E12" t="s">
         <v>190</v>
       </c>
       <c r="F12" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="G12" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -4586,13 +4732,13 @@
         <v>223</v>
       </c>
       <c r="L12" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="M12" t="s">
         <v>223</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -4669,7 +4815,7 @@
         <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
       <c r="C2" t="s">
         <v>77</v>
@@ -4716,7 +4862,7 @@
         <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="C3" t="s">
         <v>77</v>
@@ -4987,7 +5133,7 @@
         <v>77</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>77</v>
@@ -5004,19 +5150,19 @@
         <v>96</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>102</v>
@@ -5031,13 +5177,13 @@
         <v>105</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -5045,22 +5191,22 @@
         <v>162</v>
       </c>
       <c r="B10" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="C10" s="14">
         <v>45582.54724537037</v>
       </c>
       <c r="D10" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
       <c r="E10" t="s">
         <v>190</v>
       </c>
       <c r="F10" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="G10" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -5075,13 +5221,13 @@
         <v>223</v>
       </c>
       <c r="L10" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="M10" t="s">
         <v>223</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="O10" t="s">
         <v>77</v>
@@ -5092,22 +5238,22 @@
         <v>162</v>
       </c>
       <c r="B11" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="C11" s="14">
         <v>45582.54724537037</v>
       </c>
       <c r="D11" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="E11" t="s">
         <v>190</v>
       </c>
       <c r="F11" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="G11" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -5122,16 +5268,16 @@
         <v>223</v>
       </c>
       <c r="L11" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="M11" t="s">
         <v>223</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>507</v>
+        <v>494</v>
       </c>
       <c r="O11" t="s">
-        <v>506</v>
+        <v>493</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -5139,22 +5285,22 @@
         <v>162</v>
       </c>
       <c r="B12" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="C12" s="14">
         <v>45582.54724537037</v>
       </c>
       <c r="D12" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
       <c r="E12" t="s">
         <v>190</v>
       </c>
       <c r="F12" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="G12" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -5169,13 +5315,13 @@
         <v>223</v>
       </c>
       <c r="L12" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="M12" t="s">
         <v>223</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="O12" t="s">
         <v>77</v>
@@ -5195,521 +5341,587 @@
   <sheetPr>
     <tabColor theme="3" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:A100"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="255.59765625" bestFit="1"/>
+    <col min="1" max="1" width="35.69921875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="90.69921875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>517</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="22" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="3" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="20"/>
+      <c r="B3" s="23" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
+    <row r="4" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="20"/>
+      <c r="B4" s="23" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="21"/>
+      <c r="B5" s="24"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="22" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" s="23" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="20"/>
+      <c r="B8" s="23" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="21"/>
+      <c r="B9" s="24"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
+      <c r="B10" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="20"/>
+      <c r="B11" s="23" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>11</v>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="20"/>
+      <c r="B13" s="23" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="21"/>
+      <c r="B14" s="24"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
         <v>13</v>
       </c>
+      <c r="B15" s="22" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>14</v>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="20"/>
+      <c r="B16" s="23" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>15</v>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="20"/>
+      <c r="B17" s="23" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>16</v>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="23" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="21"/>
+      <c r="B19" s="24"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="19" t="s">
         <v>18</v>
       </c>
+      <c r="B20" s="22" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>19</v>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="23" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>20</v>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="23" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>21</v>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="20"/>
+      <c r="B23" s="23" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="21"/>
+      <c r="B24" s="24"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="19" t="s">
         <v>23</v>
       </c>
+      <c r="B25" s="22" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>24</v>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="20"/>
+      <c r="B26" s="23" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>25</v>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="20"/>
+      <c r="B27" s="23" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>26</v>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="20"/>
+      <c r="B28" s="23" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="21"/>
+      <c r="B29" s="24"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="19" t="s">
         <v>28</v>
       </c>
+      <c r="B30" s="22" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>29</v>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="20"/>
+      <c r="B31" s="23" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>30</v>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="20"/>
+      <c r="B32" s="23" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>31</v>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="20"/>
+      <c r="B33" s="23" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="21"/>
+      <c r="B34" s="24"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="19" t="s">
         <v>33</v>
       </c>
+      <c r="B35" s="22" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>34</v>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="20"/>
+      <c r="B36" s="23" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>35</v>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="20"/>
+      <c r="B37" s="23" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>36</v>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="20"/>
+      <c r="B38" s="23" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="21"/>
+      <c r="B39" s="24"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="19" t="s">
         <v>38</v>
       </c>
+      <c r="B40" s="22" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>39</v>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="20"/>
+      <c r="B41" s="23" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>40</v>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="20"/>
+      <c r="B42" s="23" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>41</v>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="19"/>
+      <c r="B43" s="22" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>42</v>
-      </c>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="20"/>
+      <c r="B44" s="23"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="20" t="s">
         <v>43</v>
       </c>
+      <c r="B45" s="23" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>44</v>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="20"/>
+      <c r="B46" s="23" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>45</v>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="20"/>
+      <c r="B47" s="23" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>46</v>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="20"/>
+      <c r="B48" s="23" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>47</v>
-      </c>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="21"/>
+      <c r="B49" s="24"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="50" spans="1:2" ht="78" x14ac:dyDescent="0.3">
+      <c r="A50" s="19" t="s">
         <v>48</v>
       </c>
+      <c r="B50" s="22" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="50" spans="1:1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>49</v>
-      </c>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="21"/>
+      <c r="B51" s="24"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="52" spans="1:2" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="19" t="s">
         <v>50</v>
       </c>
+      <c r="B52" s="22" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>51</v>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="20"/>
+      <c r="B53" s="23" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>52</v>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="20"/>
+      <c r="B54" s="23" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>53</v>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="20"/>
+      <c r="B55" s="23" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>54</v>
-      </c>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="21"/>
+      <c r="B56" s="24"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="57" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="19" t="s">
         <v>55</v>
       </c>
+      <c r="B57" s="22" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>56</v>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="20"/>
+      <c r="B58" s="23" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>57</v>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="20"/>
+      <c r="B59" s="23" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>58</v>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="20"/>
+      <c r="B60" s="23" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>59</v>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="21"/>
+      <c r="B61" s="24" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B89" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B91" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B93" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B95" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B96" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" s="1" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:A100" numberStoredAsText="1"/>
+    <ignoredError sqref="B2:B4 B15:B18 B10:B13 B6:B8 B20:B23 B25:B28 B30:B33 B35:B38 B40:B43 B45:B48 B50 B52:B55 B57:B100" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -6949,7 +7161,7 @@
         <v>71</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="D5" t="s">
         <v>63</v>
@@ -7248,7 +7460,7 @@
         <v>73</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="D6" t="s">
         <v>63</v>
@@ -37510,7 +37722,7 @@
   </sheetPr>
   <dimension ref="A1:BO7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -41495,22 +41707,22 @@
   </sheetPr>
   <dimension ref="A1:CV100"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="59.3984375" customWidth="1"/>
-    <col min="2" max="2" width="111.19921875" customWidth="1"/>
+    <col min="1" max="1" width="35.69921875" customWidth="1"/>
+    <col min="2" max="2" width="90.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>367</v>
+        <v>355</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>518</v>
       </c>
       <c r="C1" t="s">
         <v>63</v>
@@ -41809,10 +42021,10 @@
     </row>
     <row r="2" spans="1:100" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>365</v>
+        <v>519</v>
       </c>
       <c r="C2" t="s">
         <v>63</v>
@@ -42111,10 +42323,10 @@
     </row>
     <row r="3" spans="1:100" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>363</v>
+        <v>520</v>
       </c>
       <c r="C3" t="s">
         <v>63</v>
@@ -42413,10 +42625,10 @@
     </row>
     <row r="4" spans="1:100" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>361</v>
+        <v>521</v>
       </c>
       <c r="C4" t="s">
         <v>63</v>
@@ -42715,10 +42927,10 @@
     </row>
     <row r="5" spans="1:100" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>359</v>
+        <v>522</v>
       </c>
       <c r="C5" t="s">
         <v>63</v>
@@ -43017,10 +43229,10 @@
     </row>
     <row r="6" spans="1:100" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="C6" t="s">
         <v>63</v>
@@ -43319,10 +43531,10 @@
     </row>
     <row r="7" spans="1:100" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>355</v>
+        <v>523</v>
       </c>
       <c r="C7" t="s">
         <v>63</v>
@@ -43621,10 +43833,10 @@
     </row>
     <row r="8" spans="1:100" ht="78" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>353</v>
+        <v>524</v>
       </c>
       <c r="C8" t="s">
         <v>63</v>
@@ -43923,10 +44135,10 @@
     </row>
     <row r="9" spans="1:100" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C9" t="s">
         <v>63</v>
@@ -44225,10 +44437,10 @@
     </row>
     <row r="10" spans="1:100" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>349</v>
+        <v>525</v>
       </c>
       <c r="C10" t="s">
         <v>63</v>
@@ -44527,10 +44739,10 @@
     </row>
     <row r="11" spans="1:100" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>347</v>
+        <v>526</v>
       </c>
       <c r="C11" t="s">
         <v>63</v>
@@ -44829,10 +45041,10 @@
     </row>
     <row r="12" spans="1:100" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>345</v>
+        <v>527</v>
       </c>
       <c r="C12" t="s">
         <v>63</v>
@@ -45131,10 +45343,10 @@
     </row>
     <row r="13" spans="1:100" ht="78" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>343</v>
+        <v>528</v>
       </c>
       <c r="C13" t="s">
         <v>63</v>
@@ -45433,10 +45645,10 @@
     </row>
     <row r="14" spans="1:100" ht="78" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C14" t="s">
         <v>63</v>
@@ -45735,10 +45947,10 @@
     </row>
     <row r="15" spans="1:100" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C15" t="s">
         <v>63</v>
@@ -46037,10 +46249,10 @@
     </row>
     <row r="16" spans="1:100" ht="78" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C16" t="s">
         <v>63</v>
@@ -46339,10 +46551,10 @@
     </row>
     <row r="17" spans="1:100" ht="78" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C17" t="s">
         <v>63</v>
@@ -46641,10 +46853,10 @@
     </row>
     <row r="18" spans="1:100" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>333</v>
+        <v>529</v>
       </c>
       <c r="C18" t="s">
         <v>63</v>
@@ -46943,10 +47155,10 @@
     </row>
     <row r="19" spans="1:100" ht="78" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>331</v>
+        <v>530</v>
       </c>
       <c r="C19" t="s">
         <v>63</v>
@@ -71720,53 +71932,53 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.59765625" customWidth="1"/>
     <col min="2" max="2" width="69.69921875" customWidth="1"/>
-    <col min="3" max="3" width="27.69921875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="27.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="78" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="78" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>529</v>
+        <v>358</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>529</v>
+        <v>356</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>516</v>
       </c>
     </row>
   </sheetData>
@@ -72104,7 +72316,7 @@
         <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="C2" t="s">
         <v>77</v>
@@ -72415,7 +72627,7 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="C3" t="s">
         <v>77</v>
@@ -73982,7 +74194,7 @@
         <v>77</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>77</v>
@@ -74078,7 +74290,7 @@
         <v>77</v>
       </c>
       <c r="AL8" s="4" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="AM8" s="4" t="s">
         <v>77</v>
@@ -74096,7 +74308,7 @@
         <v>77</v>
       </c>
       <c r="AR8" s="3" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="AS8" s="3" t="s">
         <v>77</v>
@@ -74281,28 +74493,28 @@
         <v>94</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>107</v>
@@ -74314,16 +74526,16 @@
         <v>109</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="O9" s="6" t="s">
         <v>271</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="Q9" s="6" t="s">
         <v>236</v>
@@ -74332,19 +74544,19 @@
         <v>237</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="T9" s="6" t="s">
         <v>314</v>
       </c>
       <c r="U9" s="6" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="V9" s="6" t="s">
         <v>258</v>
       </c>
       <c r="W9" s="6" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="X9" s="6" t="s">
         <v>248</v>
@@ -74353,7 +74565,7 @@
         <v>256</v>
       </c>
       <c r="Z9" s="6" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="AA9" s="6" t="s">
         <v>246</v>
@@ -74377,7 +74589,7 @@
         <v>312</v>
       </c>
       <c r="AH9" s="6" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="AI9" s="6" t="s">
         <v>310</v>
@@ -74386,10 +74598,10 @@
         <v>309</v>
       </c>
       <c r="AK9" s="6" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="AL9" s="5" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="AM9" s="6" t="s">
         <v>154</v>
@@ -74407,46 +74619,46 @@
         <v>158</v>
       </c>
       <c r="AR9" s="5" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="AS9" s="5" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="AT9" s="5" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="AU9" s="5" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="AV9" s="5" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="AW9" s="5" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="AX9" s="5" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="AY9" s="5" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="AZ9" s="5" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="BA9" s="5" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="BB9" s="5" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="BC9" s="6" t="s">
         <v>308</v>
       </c>
       <c r="BD9" s="6" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="BE9" s="6" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
       <c r="BF9" s="6" t="s">
         <v>271</v>
@@ -74503,16 +74715,16 @@
         <v>289</v>
       </c>
       <c r="BX9" s="6" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="BY9" s="6" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="BZ9" s="6" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="CA9" s="6" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="CB9" s="6" t="s">
         <v>288</v>
@@ -74527,16 +74739,16 @@
         <v>285</v>
       </c>
       <c r="CF9" s="6" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="CG9" s="6" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="CH9" s="6" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="CI9" s="6" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="CJ9" s="6" t="s">
         <v>275</v>
@@ -74566,10 +74778,10 @@
         <v>266</v>
       </c>
       <c r="CS9" s="6" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="CT9" s="5" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="CU9" s="5" t="s">
         <v>242</v>
@@ -74584,72 +74796,72 @@
         <v>239</v>
       </c>
       <c r="CY9" s="5" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
     </row>
     <row r="10" spans="1:103" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="B10" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="C10" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="D10" t="s">
         <v>207</v>
       </c>
       <c r="E10" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="R10" s="11" t="s">
         <v>227</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="V10" s="11" t="s">
         <v>227</v>
@@ -74661,34 +74873,34 @@
         <v>227</v>
       </c>
       <c r="Y10" s="11" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="Z10" s="11" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="AA10" s="11" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="AB10" s="11" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="AC10" s="9" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="AD10" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="AE10" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="AF10" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="AG10" s="11" t="s">
         <v>197</v>
       </c>
       <c r="AH10" s="9" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="AI10" s="11" t="s">
         <v>227</v>
@@ -74751,73 +74963,73 @@
         <v>77</v>
       </c>
       <c r="BC10" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="BD10" s="13" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="BE10" s="12" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="BF10" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="BG10" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="BH10" t="s">
         <v>227</v>
       </c>
       <c r="BI10" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="BJ10" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="BK10" t="s">
         <v>227</v>
       </c>
       <c r="BL10" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="BM10" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="BN10" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="BO10" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="BP10" t="s">
         <v>227</v>
       </c>
       <c r="BQ10" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="BR10" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="BS10" t="s">
         <v>227</v>
       </c>
       <c r="BT10" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="BU10" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="BV10" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="BW10" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="BX10" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="BY10" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="BZ10" t="s">
         <v>227</v>
@@ -74826,16 +75038,16 @@
         <v>227</v>
       </c>
       <c r="CB10" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="CC10" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="CD10" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="CE10" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="CF10" t="s">
         <v>227</v>
@@ -74850,16 +75062,16 @@
         <v>227</v>
       </c>
       <c r="CJ10" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="CK10" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="CL10" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="CM10" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="CN10" t="s">
         <v>227</v>
@@ -74868,34 +75080,34 @@
         <v>227</v>
       </c>
       <c r="CP10" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="CQ10" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="CR10" t="s">
         <v>227</v>
       </c>
       <c r="CS10" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="CT10" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="CU10" t="s">
         <v>207</v>
       </c>
       <c r="CV10" s="9" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="CW10" s="11" t="s">
         <v>227</v>
       </c>
       <c r="CX10" s="9" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="CY10" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>